<commit_message>
updates to RdotNetConnector; updates to DataTabler
</commit_message>
<xml_diff>
--- a/BaseballScraper.xlsx
+++ b/BaseballScraper.xlsx
@@ -1,302 +1,310 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <workbookPr autoCompressPictures="1"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10814"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/DanBinder/Google_Drive/Coding/Projects/BaseballScraper/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D2ABA43-8093-2744-BF98-BA352F4718DD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView tabRatio="600"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="25600" windowHeight="14700" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="djb" sheetId="1" r:id="rId3"/>
-    <sheet name="sheet2" sheetId="2" r:id="rId4"/>
-    <sheet name="ninja" sheetId="3" r:id="rId5"/>
-    <sheet name="popcorn" sheetId="4" r:id="rId6"/>
-    <sheet name="FgHitters" sheetId="5" r:id="rId7"/>
-    <sheet name="FgHitter" sheetId="6" r:id="rId8"/>
+    <sheet name="djb" sheetId="1" r:id="rId1"/>
+    <sheet name="sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="ninja" sheetId="3" r:id="rId3"/>
+    <sheet name="popcorn" sheetId="4" r:id="rId4"/>
+    <sheet name="FgHitters" sheetId="5" r:id="rId5"/>
+    <sheet name="FgHitter" sheetId="6" r:id="rId6"/>
   </sheets>
+  <calcPr calcId="0" calcCompleted="0" calcOnSave="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="332" uniqueCount="91">
   <si>
-    <t xml:space="preserve">RecordNumber</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FanGraphsName</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FanGraphsTeam</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FanGraphsAge</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GamesStarted</t>
-  </si>
-  <si>
-    <t xml:space="preserve">InningsPitched</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TotalBattersFaced</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Wins</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Saves</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ks</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Holds</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Era</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Whip</t>
-  </si>
-  <si>
-    <t xml:space="preserve">StrikeoutPercentage</t>
-  </si>
-  <si>
-    <t xml:space="preserve">WalkPercentage</t>
-  </si>
-  <si>
-    <t xml:space="preserve">StrikeoutsMinusWalks</t>
-  </si>
-  <si>
-    <t xml:space="preserve">StrikeoutsPer9</t>
-  </si>
-  <si>
-    <t xml:space="preserve">WalksPer9</t>
-  </si>
-  <si>
-    <t xml:space="preserve">StrikeoutsDividedByWalks</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Balls</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Strikes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pitches</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HomeRunsPer9</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GroundballPercent</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LinedrivePercent</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FlyballPercent</t>
-  </si>
-  <si>
-    <t xml:space="preserve">InfieldFlyballPercent</t>
-  </si>
-  <si>
-    <t xml:space="preserve">OSwingPercent</t>
-  </si>
-  <si>
-    <t xml:space="preserve">OSwingPercentPfx</t>
-  </si>
-  <si>
-    <t xml:space="preserve">OSwingPercentPi</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ZContactPercent</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ZContactPercentPfx</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ZContactPercentPi</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ContactPercent</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ContactPercentPfx</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ContactPercentPi</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ZonePercent</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ZonePercentPfx</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ZonePercentPi</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FStrikePercent</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SwStrPercent</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PullPercent</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SoftPercent</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sHardPercent</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Babip</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LeftOnBasePercent</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HomerunsDividedByFlyballs</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FastballVelocityPfx</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EraRepeat</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EraMinus</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fip</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FipMinus</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EraMinusFip</t>
-  </si>
-  <si>
-    <t xml:space="preserve">XFip</t>
-  </si>
-  <si>
-    <t xml:space="preserve">XFipMinus</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Siera</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RunsPer9</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FanGraphsId</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GP</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RBI</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SB</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BB_percent</t>
-  </si>
-  <si>
-    <t xml:space="preserve">K_percent</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ISO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BABIP</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AVG</t>
-  </si>
-  <si>
-    <t xml:space="preserve">OBP</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SLG</t>
-  </si>
-  <si>
-    <t xml:space="preserve">wOBA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">wRC_plus</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BsR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Off</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Def</t>
-  </si>
-  <si>
-    <t xml:space="preserve">WAR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Javier Baez</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Chicago Cubs</t>
-  </si>
-  <si>
-    <t xml:space="preserve">123</t>
-  </si>
-  <si>
-    <t xml:space="preserve">23%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">.321</t>
-  </si>
-  <si>
-    <t xml:space="preserve">789</t>
-  </si>
-  <si>
-    <t xml:space="preserve">6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Kris Bryant</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Anthony Rizzo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ben Zobrist</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Daniel Murphy</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tommy LaStella</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Addison Russell</t>
-  </si>
-  <si>
-    <t xml:space="preserve">David Bote</t>
+    <t>RecordNumber</t>
+  </si>
+  <si>
+    <t>FanGraphsName</t>
+  </si>
+  <si>
+    <t>FanGraphsTeam</t>
+  </si>
+  <si>
+    <t>FanGraphsAge</t>
+  </si>
+  <si>
+    <t>GamesStarted</t>
+  </si>
+  <si>
+    <t>InningsPitched</t>
+  </si>
+  <si>
+    <t>TotalBattersFaced</t>
+  </si>
+  <si>
+    <t>Wins</t>
+  </si>
+  <si>
+    <t>Saves</t>
+  </si>
+  <si>
+    <t>Ks</t>
+  </si>
+  <si>
+    <t>Holds</t>
+  </si>
+  <si>
+    <t>Era</t>
+  </si>
+  <si>
+    <t>Whip</t>
+  </si>
+  <si>
+    <t>StrikeoutPercentage</t>
+  </si>
+  <si>
+    <t>WalkPercentage</t>
+  </si>
+  <si>
+    <t>StrikeoutsMinusWalks</t>
+  </si>
+  <si>
+    <t>StrikeoutsPer9</t>
+  </si>
+  <si>
+    <t>WalksPer9</t>
+  </si>
+  <si>
+    <t>StrikeoutsDividedByWalks</t>
+  </si>
+  <si>
+    <t>Balls</t>
+  </si>
+  <si>
+    <t>Strikes</t>
+  </si>
+  <si>
+    <t>Pitches</t>
+  </si>
+  <si>
+    <t>HomeRunsPer9</t>
+  </si>
+  <si>
+    <t>GroundballPercent</t>
+  </si>
+  <si>
+    <t>LinedrivePercent</t>
+  </si>
+  <si>
+    <t>FlyballPercent</t>
+  </si>
+  <si>
+    <t>InfieldFlyballPercent</t>
+  </si>
+  <si>
+    <t>OSwingPercent</t>
+  </si>
+  <si>
+    <t>OSwingPercentPfx</t>
+  </si>
+  <si>
+    <t>OSwingPercentPi</t>
+  </si>
+  <si>
+    <t>ZContactPercent</t>
+  </si>
+  <si>
+    <t>ZContactPercentPfx</t>
+  </si>
+  <si>
+    <t>ZContactPercentPi</t>
+  </si>
+  <si>
+    <t>ContactPercent</t>
+  </si>
+  <si>
+    <t>ContactPercentPfx</t>
+  </si>
+  <si>
+    <t>ContactPercentPi</t>
+  </si>
+  <si>
+    <t>ZonePercent</t>
+  </si>
+  <si>
+    <t>ZonePercentPfx</t>
+  </si>
+  <si>
+    <t>ZonePercentPi</t>
+  </si>
+  <si>
+    <t>FStrikePercent</t>
+  </si>
+  <si>
+    <t>SwStrPercent</t>
+  </si>
+  <si>
+    <t>PullPercent</t>
+  </si>
+  <si>
+    <t>SoftPercent</t>
+  </si>
+  <si>
+    <t>sHardPercent</t>
+  </si>
+  <si>
+    <t>Babip</t>
+  </si>
+  <si>
+    <t>LeftOnBasePercent</t>
+  </si>
+  <si>
+    <t>HomerunsDividedByFlyballs</t>
+  </si>
+  <si>
+    <t>FastballVelocityPfx</t>
+  </si>
+  <si>
+    <t>EraRepeat</t>
+  </si>
+  <si>
+    <t>EraMinus</t>
+  </si>
+  <si>
+    <t>Fip</t>
+  </si>
+  <si>
+    <t>FipMinus</t>
+  </si>
+  <si>
+    <t>EraMinusFip</t>
+  </si>
+  <si>
+    <t>XFip</t>
+  </si>
+  <si>
+    <t>XFipMinus</t>
+  </si>
+  <si>
+    <t>Siera</t>
+  </si>
+  <si>
+    <t>RunsPer9</t>
+  </si>
+  <si>
+    <t>FanGraphsId</t>
+  </si>
+  <si>
+    <t>GP</t>
+  </si>
+  <si>
+    <t>PA</t>
+  </si>
+  <si>
+    <t>HR</t>
+  </si>
+  <si>
+    <t>R</t>
+  </si>
+  <si>
+    <t>RBI</t>
+  </si>
+  <si>
+    <t>SB</t>
+  </si>
+  <si>
+    <t>BB_percent</t>
+  </si>
+  <si>
+    <t>K_percent</t>
+  </si>
+  <si>
+    <t>ISO</t>
+  </si>
+  <si>
+    <t>BABIP</t>
+  </si>
+  <si>
+    <t>AVG</t>
+  </si>
+  <si>
+    <t>OBP</t>
+  </si>
+  <si>
+    <t>SLG</t>
+  </si>
+  <si>
+    <t>wOBA</t>
+  </si>
+  <si>
+    <t>wRC_plus</t>
+  </si>
+  <si>
+    <t>BsR</t>
+  </si>
+  <si>
+    <t>Off</t>
+  </si>
+  <si>
+    <t>Def</t>
+  </si>
+  <si>
+    <t>WAR</t>
+  </si>
+  <si>
+    <t>Javier Baez</t>
+  </si>
+  <si>
+    <t>Chicago Cubs</t>
+  </si>
+  <si>
+    <t>123</t>
+  </si>
+  <si>
+    <t>23%</t>
+  </si>
+  <si>
+    <t>.321</t>
+  </si>
+  <si>
+    <t>789</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>Kris Bryant</t>
+  </si>
+  <si>
+    <t>Anthony Rizzo</t>
+  </si>
+  <si>
+    <t>Ben Zobrist</t>
+  </si>
+  <si>
+    <t>Daniel Murphy</t>
+  </si>
+  <si>
+    <t>Tommy LaStella</t>
+  </si>
+  <si>
+    <t>Addison Russell</t>
+  </si>
+  <si>
+    <t>David Bote</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -310,7 +318,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="darkGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
   <borders count="1">
@@ -323,23 +331,331 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
+  <cellStyles count="1">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+  </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="44546A"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E7E6E6"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4472C4"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="ED7D31"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="A5A5A5"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="FFC000"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="5B9BD5"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="70AD47"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0563C1"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="954F72"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:BE1"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="1" showOutlineSymbols="1" defaultGridColor="1" colorId="64" zoomScale="100" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -511,65 +827,6 @@
       <c r="BE1" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="2">
-      <c r="A2"/>
-      <c r="B2"/>
-      <c r="C2"/>
-      <c r="D2"/>
-      <c r="E2"/>
-      <c r="F2"/>
-      <c r="G2"/>
-      <c r="H2"/>
-      <c r="I2"/>
-      <c r="J2"/>
-      <c r="K2"/>
-      <c r="L2"/>
-      <c r="M2"/>
-      <c r="N2"/>
-      <c r="O2"/>
-      <c r="P2"/>
-      <c r="Q2"/>
-      <c r="R2"/>
-      <c r="S2"/>
-      <c r="T2"/>
-      <c r="U2"/>
-      <c r="V2"/>
-      <c r="W2"/>
-      <c r="X2"/>
-      <c r="Y2"/>
-      <c r="Z2"/>
-      <c r="AA2"/>
-      <c r="AB2"/>
-      <c r="AC2"/>
-      <c r="AD2"/>
-      <c r="AE2"/>
-      <c r="AF2"/>
-      <c r="AG2"/>
-      <c r="AH2"/>
-      <c r="AI2"/>
-      <c r="AJ2"/>
-      <c r="AK2"/>
-      <c r="AL2"/>
-      <c r="AM2"/>
-      <c r="AN2"/>
-      <c r="AO2"/>
-      <c r="AP2"/>
-      <c r="AQ2"/>
-      <c r="AR2"/>
-      <c r="AS2"/>
-      <c r="AT2"/>
-      <c r="AU2"/>
-      <c r="AV2"/>
-      <c r="AW2"/>
-      <c r="AX2"/>
-      <c r="AY2"/>
-      <c r="AZ2"/>
-      <c r="BA2"/>
-      <c r="BB2"/>
-      <c r="BC2"/>
-      <c r="BD2"/>
-      <c r="BE2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -577,50 +834,52 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView showRuler="1" showOutlineSymbols="1" defaultGridColor="1" colorId="64" zoomScale="100" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView showRuler="1" showOutlineSymbols="1" defaultGridColor="1" colorId="64" zoomScale="100" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView showRuler="1" showOutlineSymbols="1" defaultGridColor="1" colorId="64" zoomScale="100" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+  <dimension ref="A1:V11"/>
   <sheetViews>
-    <sheetView showRuler="1" showOutlineSymbols="1" defaultGridColor="1" colorId="64" zoomScale="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>57</v>
       </c>
@@ -688,8 +947,10 @@
         <v>76</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2"/>
+    <row r="2" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1</v>
+      </c>
       <c r="B2" t="s">
         <v>77</v>
       </c>
@@ -754,8 +1015,10 @@
         <v>83</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3"/>
+    <row r="3" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>2</v>
+      </c>
       <c r="B3" t="s">
         <v>84</v>
       </c>
@@ -820,8 +1083,10 @@
         <v>83</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4"/>
+    <row r="4" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>3</v>
+      </c>
       <c r="B4" t="s">
         <v>85</v>
       </c>
@@ -886,8 +1151,10 @@
         <v>83</v>
       </c>
     </row>
-    <row r="5">
-      <c r="A5"/>
+    <row r="5" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>4</v>
+      </c>
       <c r="B5" t="s">
         <v>86</v>
       </c>
@@ -952,8 +1219,10 @@
         <v>83</v>
       </c>
     </row>
-    <row r="6">
-      <c r="A6"/>
+    <row r="6" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>5</v>
+      </c>
       <c r="B6" t="s">
         <v>86</v>
       </c>
@@ -1018,8 +1287,10 @@
         <v>83</v>
       </c>
     </row>
-    <row r="7">
-      <c r="A7"/>
+    <row r="7" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>6</v>
+      </c>
       <c r="B7" t="s">
         <v>86</v>
       </c>
@@ -1084,8 +1355,10 @@
         <v>83</v>
       </c>
     </row>
-    <row r="8">
-      <c r="A8"/>
+    <row r="8" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>7</v>
+      </c>
       <c r="B8" t="s">
         <v>87</v>
       </c>
@@ -1150,8 +1423,10 @@
         <v>83</v>
       </c>
     </row>
-    <row r="9">
-      <c r="A9"/>
+    <row r="9" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>8</v>
+      </c>
       <c r="B9" t="s">
         <v>88</v>
       </c>
@@ -1216,8 +1491,10 @@
         <v>83</v>
       </c>
     </row>
-    <row r="10">
-      <c r="A10"/>
+    <row r="10" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>9</v>
+      </c>
       <c r="B10" t="s">
         <v>89</v>
       </c>
@@ -1282,8 +1559,10 @@
         <v>83</v>
       </c>
     </row>
-    <row r="11">
-      <c r="A11"/>
+    <row r="11" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>10</v>
+      </c>
       <c r="B11" t="s">
         <v>90</v>
       </c>
@@ -1354,14 +1633,14 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+  <dimension ref="A1:V2"/>
   <sheetViews>
-    <sheetView showRuler="1" showOutlineSymbols="1" defaultGridColor="1" colorId="64" zoomScale="100" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>57</v>
       </c>
@@ -1429,8 +1708,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2"/>
+    <row r="2" spans="1:22" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
         <v>85</v>
       </c>

</xml_diff>